<commit_message>
Update the comment under ReportExplorer folder.
</commit_message>
<xml_diff>
--- a/Work Documents/Forerunner V3-JS Comments Review.xlsx
+++ b/Work Documents/Forerunner V3-JS Comments Review.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="57">
   <si>
     <t>File Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -208,6 +208,44 @@
   </si>
   <si>
     <t>SubscriptionModel.js</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Not public</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Done. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>layoutReport/replayRespTablix/isNull</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Done. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ToggleItem(scrollID)</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -228,41 +266,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Not public</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Done. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>layoutReport/replayRespTablix/isNull</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Done. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ToggleItem(scrollID)</t>
-    </r>
+    <t>Baotong</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Done</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Done. transitionToReportViewer(params, urlOption)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jon</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -700,8 +716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -857,15 +873,21 @@
       <c r="B17" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
+      <c r="C17" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="18" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12"/>
       <c r="B18" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="7"/>
+      <c r="C18" s="6" t="s">
+        <v>56</v>
+      </c>
       <c r="D18" s="7"/>
     </row>
     <row r="19" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -873,56 +895,84 @@
       <c r="B19" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
+      <c r="C19" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="20" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12"/>
       <c r="B20" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
+      <c r="C20" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="21" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12"/>
       <c r="B21" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
+      <c r="C21" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="22" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
       <c r="B22" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
+      <c r="C22" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="23" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12"/>
       <c r="B23" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
+      <c r="C23" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="24" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
       <c r="B24" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
+      <c r="C24" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="25" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12"/>
       <c r="B25" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
+      <c r="C25" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="26" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
@@ -1031,7 +1081,7 @@
         <v>46</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1043,7 +1093,7 @@
         <v>46</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1067,7 +1117,7 @@
         <v>46</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1079,7 +1129,7 @@
         <v>46</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update the comment under Common folder.
</commit_message>
<xml_diff>
--- a/Work Documents/Forerunner V3-JS Comments Review.xlsx
+++ b/Work Documents/Forerunner V3-JS Comments Review.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="60">
   <si>
     <t>File Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -208,10 +208,6 @@
   </si>
   <si>
     <t>SubscriptionModel.js</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Not public</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -249,23 +245,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Done. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>getSchedules (return type?)</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Baotong</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -278,7 +257,27 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Jon</t>
+    <t>Private</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Private</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Baotong</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>private</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Baotong</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Done</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -716,8 +715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -749,72 +748,108 @@
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
+      <c r="C2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A3" s="10"/>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
+      <c r="C3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A4" s="10"/>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="C4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A5" s="10"/>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
+      <c r="C5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A6" s="10"/>
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
+      <c r="C6" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A7" s="10"/>
       <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
+      <c r="C7" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A8" s="10"/>
       <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+      <c r="C8" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A9" s="10"/>
       <c r="B9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
+      <c r="C9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A10" s="10"/>
       <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
+      <c r="C10" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
@@ -874,10 +909,10 @@
         <v>24</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -886,9 +921,11 @@
         <v>25</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D18" s="7"/>
+        <v>58</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="19" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
@@ -896,10 +933,10 @@
         <v>26</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -908,10 +945,10 @@
         <v>27</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -920,10 +957,10 @@
         <v>28</v>
       </c>
       <c r="C21" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="7" t="s">
         <v>53</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -932,10 +969,10 @@
         <v>29</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -944,10 +981,10 @@
         <v>30</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -956,10 +993,10 @@
         <v>31</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -968,10 +1005,10 @@
         <v>32</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1081,7 +1118,7 @@
         <v>46</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1093,7 +1130,7 @@
         <v>46</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1117,7 +1154,7 @@
         <v>46</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1126,10 +1163,10 @@
         <v>48</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>